<commit_message>
Create sim params for 12 species
</commit_message>
<xml_diff>
--- a/data/small/interacting_pairs_per_survey_with_interactions.xlsx
+++ b/data/small/interacting_pairs_per_survey_with_interactions.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\Deepbios\data\small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9B1455C-5BEC-4DA2-AEC2-45CD5B21F996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E816782D-E780-4906-86AC-3C192FFE9DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="4395" windowWidth="20910" windowHeight="11595" xr2:uid="{9E08221B-A731-4435-ACB0-20454CBDE701}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="18465" windowHeight="10996" activeTab="2" xr2:uid="{9E08221B-A731-4435-ACB0-20454CBDE701}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="food sources" sheetId="2" r:id="rId2"/>
+    <sheet name="interactions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
   <si>
     <t>child</t>
   </si>
@@ -106,14 +108,61 @@
   </si>
   <si>
     <t>Interaction</t>
+  </si>
+  <si>
+    <t>Food sources</t>
+  </si>
+  <si>
+    <t>Platichthys flesus</t>
+  </si>
+  <si>
+    <t>Aphia minuta</t>
+  </si>
+  <si>
+    <t>Chelidonichthys cuculus</t>
+  </si>
+  <si>
+    <t>Dicentrarchus labrax</t>
+  </si>
+  <si>
+    <t>Scophthalmus rhombus</t>
+  </si>
+  <si>
+    <t>Trachinus draco</t>
+  </si>
+  <si>
+    <t>Hippoglossoides platessoides</t>
+  </si>
+  <si>
+    <t>Lumpenus lampretaeformis</t>
+  </si>
+  <si>
+    <t>Lycodes vahlii</t>
+  </si>
+  <si>
+    <t>Enchelyopus cimbrius</t>
+  </si>
+  <si>
+    <t>Lycenchelys sarsii</t>
+  </si>
+  <si>
+    <t>Interactions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,8 +190,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,13 +509,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A012907-776A-4034-86E4-67A167B2ED04}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -493,7 +549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -507,7 +563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -521,7 +577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -535,7 +591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -549,7 +605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -563,7 +619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -577,7 +633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -591,7 +647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -605,7 +661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -619,7 +675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -633,7 +689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -647,7 +703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -659,6 +715,1109 @@
       </c>
       <c r="D14" t="s">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E6E259-F06B-4F05-8019-C2BCF720694C}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="A1:M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FA47DE-7DB4-4C9A-BDB2-6344CF81EB08}">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="A1:M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>